<commit_message>
added friendly tab name to links field
</commit_message>
<xml_diff>
--- a/examples/template/generic.xlsx
+++ b/examples/template/generic.xlsx
@@ -3005,10 +3005,10 @@
     <t>specimen_from_organism.purchased_specimen.kit_titer</t>
   </si>
   <si>
-    <t>DERIVED FROM  donor_organism</t>
-  </si>
-  <si>
-    <t>Enter biomaterial ID from specimen_from_organism tab that this biomaterial was derrived from.</t>
+    <t>DERIVED FROM SPECIMEN FROM ORGANISM</t>
+  </si>
+  <si>
+    <t>Enter biomaterial ID from Specimen from organism tab that this biomaterial was derrived from.</t>
   </si>
   <si>
     <t>donor_organism.biomaterial_core.biomaterial_id</t>
@@ -3314,10 +3314,10 @@
     <t>cell_suspension.plate_based_sequencing.cell_quality</t>
   </si>
   <si>
-    <t>DERIVED FROM  specimen_from_organism</t>
-  </si>
-  <si>
-    <t>Enter biomaterial ID from cell_suspension tab that this biomaterial was derrived from.</t>
+    <t>DERIVED FROM CELL SUSPENSION</t>
+  </si>
+  <si>
+    <t>Enter biomaterial ID from Cell suspension tab that this biomaterial was derrived from.</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
added first attempt at example filling
</commit_message>
<xml_diff>
--- a/examples/template/generic.xlsx
+++ b/examples/template/generic.xlsx
@@ -891,18 +891,18 @@
     <t>sequence_file.library_prep_id</t>
   </si>
   <si>
+    <t>SEQUENCING PROTOCOL</t>
+  </si>
+  <si>
+    <t>Enter protocol ID from SEQUENCING PROTOCOL tab that this entity was derrived from.</t>
+  </si>
+  <si>
     <t>LIBRARY PREPARATION PROTOCOL</t>
   </si>
   <si>
     <t>Enter protocol ID from LIBRARY PREPARATION PROTOCOL tab that this entity was derrived from.</t>
   </si>
   <si>
-    <t>SEQUENCING PROTOCOL</t>
-  </si>
-  <si>
-    <t>Enter protocol ID from SEQUENCING PROTOCOL tab that this entity was derrived from.</t>
-  </si>
-  <si>
     <t>DERIVED FROM CELL SUSPENSION</t>
   </si>
   <si>
@@ -2181,16 +2181,16 @@
     <t>cell_suspension.plate_based_sequencing.cell_quality</t>
   </si>
   <si>
+    <t>ENRICHMENT PROTOCOL</t>
+  </si>
+  <si>
+    <t>Enter protocol ID from ENRICHMENT PROTOCOL tab that this entity was derrived from.</t>
+  </si>
+  <si>
     <t>DISSOCIATION PROTOCOL</t>
   </si>
   <si>
     <t>Enter protocol ID from DISSOCIATION PROTOCOL tab that this entity was derrived from.</t>
-  </si>
-  <si>
-    <t>ENRICHMENT PROTOCOL</t>
-  </si>
-  <si>
-    <t>Enter protocol ID from ENRICHMENT PROTOCOL tab that this entity was derrived from.</t>
   </si>
   <si>
     <t>DERIVED FROM SPECIMEN FROM ORGANISM</t>
@@ -4364,10 +4364,10 @@
         <v>288</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>3</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>295</v>
@@ -6459,10 +6459,10 @@
         <v>718</v>
       </c>
       <c r="AK4" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="AL4" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="AL4" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="AM4" s="3" t="s">
         <v>298</v>

</xml_diff>